<commit_message>
esta si es la version final probada en producción de la página web de la universidad
</commit_message>
<xml_diff>
--- a/Estructura Nuevo Calendario final.xlsx
+++ b/Estructura Nuevo Calendario final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conta\OneDrive - Universidad del rosario\calendario academico 2020 nuevo diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3E36B49-19AD-4B78-AA0E-67D8A4FA9C87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16003727-C6EF-4AB6-81B8-B898A4348C8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3799,10 +3799,10 @@
     <t>programa</t>
   </si>
   <si>
-    <t xml:space="preserve">categoria </t>
-  </si>
-  <si>
     <t>contenido</t>
+  </si>
+  <si>
+    <t>categoria</t>
   </si>
 </sst>
 </file>
@@ -4049,10 +4049,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4354,8 +4350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4401,10 +4397,10 @@
         <v>268</v>
       </c>
       <c r="I1" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>269</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>270</v>
       </c>
       <c r="S1" s="18"/>
     </row>

</xml_diff>